<commit_message>
加 Organ Bike 到夢 2 板
</commit_message>
<xml_diff>
--- a/MPC82/PitchTable.xlsx
+++ b/MPC82/PitchTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="480" windowWidth="18015" windowHeight="8325"/>
@@ -15,12 +15,12 @@
     <sheet name="廠商名錄" sheetId="6" r:id="rId6"/>
     <sheet name="工作表6" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="721">
   <si>
     <t>C調</t>
   </si>
@@ -4735,6 +4735,238 @@
   </si>
   <si>
     <t>上刷 i57</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Organ Bike</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(P17)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2(P20)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3(P21)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(P22)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5(P23)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>6(P24)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>7(P25)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8(P26)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9(P56)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10(P55)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>11(P34)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>12(P35)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>13(P36)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14(P37)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>15(P40)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>16(P41)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>17(P42)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>18(P43)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>19(P46)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20(P50)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>21(P51)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>22(P52)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>23(P53)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>24(P54)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>25(P00)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>26(P01)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>27(P02)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>28(P03)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>29(P04)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>30(P05)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>31(P06)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>32(P07)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>33(P11)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>34(P14)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>35(P15)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>36(P16)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>37(P17)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>38(P20)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>39(P21)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40(P22)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>41(P23)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>42(P24)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>43(P25)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>44(P26)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>45(P56)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>46(P55)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>47(P34)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>48(P35)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>49(P36)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>50(P37)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>51(P40)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>52(P41)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>53(P42)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>54(P43)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>55(P46)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>56(P50)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>57(P51)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -4790,7 +5022,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4902,6 +5134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5097,7 +5335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5274,6 +5512,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5569,13 +5843,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:S86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H48" sqref="H48"/>
+      <selection pane="bottomRight" activeCell="P72" sqref="P72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -5588,9 +5862,10 @@
     <col min="11" max="13" width="8.7109375" customWidth="1"/>
     <col min="14" max="14" width="22.5703125" customWidth="1"/>
     <col min="15" max="15" width="29.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="12.75" customHeight="1">
+    <row r="1" spans="1:19" ht="12.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -5634,11 +5909,14 @@
         <v>11</v>
       </c>
       <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="P1" s="6" t="s">
+        <v>663</v>
+      </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
-    </row>
-    <row r="2" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19" ht="12.75" customHeight="1">
       <c r="A2" s="51" t="s">
         <v>12</v>
       </c>
@@ -5680,13 +5958,14 @@
         <v>9</v>
       </c>
       <c r="O2" s="6"/>
-      <c r="P2" s="14">
+      <c r="P2" s="62"/>
+      <c r="Q2" s="14">
         <v>35</v>
       </c>
-      <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S2" s="6"/>
+    </row>
+    <row r="3" spans="1:19" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>138</v>
       </c>
@@ -5716,18 +5995,19 @@
         <v>473</v>
       </c>
       <c r="O3" s="16"/>
-      <c r="P3" s="6">
-        <f>P2+1</f>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="6">
+        <f>Q2+1</f>
         <v>36</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12.75" customHeight="1">
+    <row r="4" spans="1:19" ht="12.75" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="13" t="s">
         <v>140</v>
@@ -5772,18 +6052,21 @@
       <c r="O4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" ref="P4:P67" si="0">P3+1</f>
+      <c r="P4" s="59">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="6">
+        <f t="shared" ref="Q4:Q67" si="0">Q3+1</f>
         <v>37</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.75" customHeight="1">
+    <row r="5" spans="1:19" ht="12.75" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>142</v>
       </c>
@@ -5814,18 +6097,19 @@
         <v>475</v>
       </c>
       <c r="O5" s="16"/>
-      <c r="P5" s="6">
+      <c r="P5" s="59"/>
+      <c r="Q5" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12.75" customHeight="1">
+    <row r="6" spans="1:19" ht="12.75" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
         <v>144</v>
@@ -5856,18 +6140,19 @@
         <v>476</v>
       </c>
       <c r="O6" s="16"/>
-      <c r="P6" s="6">
+      <c r="P6" s="59"/>
+      <c r="Q6" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="R6" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="12.75" customHeight="1">
+    <row r="7" spans="1:19" ht="12.75" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>147</v>
       </c>
@@ -5900,18 +6185,19 @@
         <v>477</v>
       </c>
       <c r="O7" s="16"/>
-      <c r="P7" s="6">
+      <c r="P7" s="59"/>
+      <c r="Q7" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="12.75" customHeight="1">
+    <row r="8" spans="1:19" ht="12.75" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>148</v>
       </c>
@@ -5944,18 +6230,19 @@
         <v>478</v>
       </c>
       <c r="O8" s="16"/>
-      <c r="P8" s="6">
+      <c r="P8" s="59"/>
+      <c r="Q8" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="12.75" customHeight="1">
+    <row r="9" spans="1:19" ht="12.75" customHeight="1">
       <c r="A9" s="13"/>
       <c r="B9" s="13" t="s">
         <v>149</v>
@@ -5988,18 +6275,19 @@
         <v>479</v>
       </c>
       <c r="O9" s="16"/>
-      <c r="P9" s="6">
+      <c r="P9" s="59"/>
+      <c r="Q9" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="R9" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12.75" customHeight="1">
+    <row r="10" spans="1:19" ht="12.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>150</v>
       </c>
@@ -6032,18 +6320,19 @@
         <v>480</v>
       </c>
       <c r="O10" s="16"/>
-      <c r="P10" s="6">
+      <c r="P10" s="59"/>
+      <c r="Q10" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="R10" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="S10" s="6" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="12.75" customHeight="1">
+    <row r="11" spans="1:19" ht="12.75" customHeight="1">
       <c r="A11" s="13"/>
       <c r="B11" s="13" t="s">
         <v>151</v>
@@ -6076,18 +6365,19 @@
         <v>481</v>
       </c>
       <c r="O11" s="16"/>
-      <c r="P11" s="6">
+      <c r="P11" s="59"/>
+      <c r="Q11" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="R11" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="S11" s="6" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12.75" customHeight="1">
+    <row r="12" spans="1:19" ht="12.75" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>152</v>
       </c>
@@ -6120,18 +6410,19 @@
         <v>653</v>
       </c>
       <c r="O12" s="24"/>
-      <c r="P12" s="6">
+      <c r="P12" s="59"/>
+      <c r="Q12" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="Q12" s="6" t="s">
+      <c r="R12" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="S12" s="6" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12.75" customHeight="1">
+    <row r="13" spans="1:19" ht="12.75" customHeight="1">
       <c r="A13" s="13"/>
       <c r="B13" s="13" t="s">
         <v>154</v>
@@ -6166,18 +6457,19 @@
       <c r="O13" s="52" t="s">
         <v>654</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="60"/>
+      <c r="Q13" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="R13" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="S13" s="6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12.75" customHeight="1">
+    <row r="14" spans="1:19" ht="12.75" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>155</v>
       </c>
@@ -6210,18 +6502,19 @@
         <v>483</v>
       </c>
       <c r="O14" s="53"/>
-      <c r="P14" s="6">
+      <c r="P14" s="61"/>
+      <c r="Q14" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="R14" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="R14" s="6" t="s">
+      <c r="S14" s="6" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12.75" customHeight="1">
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -6248,18 +6541,21 @@
         <v>484</v>
       </c>
       <c r="O15" s="53"/>
-      <c r="P15" s="6">
+      <c r="P15" s="63" t="s">
+        <v>664</v>
+      </c>
+      <c r="Q15" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="R15" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="R15" s="6" t="s">
+      <c r="S15" s="6" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="12.75" customHeight="1">
+    <row r="16" spans="1:19" ht="12.75" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -6283,18 +6579,21 @@
         <v>485</v>
       </c>
       <c r="O16" s="54"/>
-      <c r="P16" s="6">
+      <c r="P16" s="63" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q16" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="Q16" s="6" t="s">
+      <c r="R16" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="R16" s="6" t="s">
+      <c r="S16" s="6" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="12.75" customHeight="1">
+    <row r="17" spans="1:19" ht="12.75" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -6321,18 +6620,21 @@
         <v>486</v>
       </c>
       <c r="O17" s="7"/>
-      <c r="P17" s="6">
+      <c r="P17" s="64" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q17" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="R17" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="R17" s="6" t="s">
+      <c r="S17" s="6" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="12.75" customHeight="1">
+    <row r="18" spans="1:19" ht="12.75" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>20</v>
@@ -6357,16 +6659,19 @@
         <v>487</v>
       </c>
       <c r="O18" s="16"/>
-      <c r="P18" s="6">
+      <c r="P18" s="64" t="s">
+        <v>667</v>
+      </c>
+      <c r="Q18" s="6">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="R18" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="R18" s="6"/>
-    </row>
-    <row r="19" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" ht="12.75" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
@@ -6397,16 +6702,19 @@
         <v>488</v>
       </c>
       <c r="O19" s="16"/>
-      <c r="P19" s="6">
+      <c r="P19" s="64" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q19" s="6">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="Q19" s="6" t="s">
+      <c r="R19" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="R19" s="6"/>
-    </row>
-    <row r="20" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" ht="12.75" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -6441,16 +6749,19 @@
         <v>489</v>
       </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="6">
+      <c r="P20" s="65" t="s">
+        <v>669</v>
+      </c>
+      <c r="Q20" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="R20" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" ht="12.75" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>27</v>
@@ -6485,16 +6796,19 @@
         <v>490</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="6">
+      <c r="P21" s="65" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q21" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="Q21" s="6" t="s">
+      <c r="R21" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:19" ht="12.75" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
@@ -6529,16 +6843,19 @@
         <v>496</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="6">
+      <c r="P22" s="65" t="s">
+        <v>671</v>
+      </c>
+      <c r="Q22" s="6">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="Q22" s="6" t="s">
+      <c r="R22" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="R22" s="6"/>
-    </row>
-    <row r="23" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:19" ht="12.75" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
         <v>31</v>
@@ -6573,18 +6890,21 @@
         <v>498</v>
       </c>
       <c r="O23" s="1"/>
-      <c r="P23" s="6">
+      <c r="P23" s="65" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q23" s="6">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="Q23" s="35" t="s">
+      <c r="R23" s="35" t="s">
         <v>652</v>
       </c>
-      <c r="R23" s="6" t="s">
+      <c r="S23" s="6" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="12.75" customHeight="1">
+    <row r="24" spans="1:19" ht="12.75" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
@@ -6619,18 +6939,21 @@
         <v>497</v>
       </c>
       <c r="O24" s="40"/>
-      <c r="P24" s="6">
+      <c r="P24" s="66" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q24" s="6">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="Q24" s="35" t="s">
+      <c r="R24" s="35" t="s">
         <v>648</v>
       </c>
-      <c r="R24" s="6" t="s">
+      <c r="S24" s="6" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="12.75" customHeight="1">
+    <row r="25" spans="1:19" ht="12.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>35</v>
@@ -6665,18 +6988,21 @@
         <v>499</v>
       </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="6">
+      <c r="P25" s="65" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q25" s="6">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="Q25" s="6" t="s">
+      <c r="R25" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="R25" s="6" t="s">
+      <c r="S25" s="6" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="12.75" customHeight="1">
+    <row r="26" spans="1:19" ht="12.75" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>38</v>
       </c>
@@ -6711,18 +7037,21 @@
         <v>500</v>
       </c>
       <c r="O26" s="1"/>
-      <c r="P26" s="6">
+      <c r="P26" s="65" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q26" s="6">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="Q26" s="6" t="s">
+      <c r="R26" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="R26" s="6" t="s">
+      <c r="S26" s="6" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="12.75" customHeight="1">
+    <row r="27" spans="1:19" ht="12.75" customHeight="1">
       <c r="A27" s="13" t="s">
         <v>40</v>
       </c>
@@ -6760,18 +7089,21 @@
         <v>491</v>
       </c>
       <c r="O27" s="1"/>
-      <c r="P27" s="6">
+      <c r="P27" s="65" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q27" s="6">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="Q27" s="6" t="s">
+      <c r="R27" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="R27" s="6" t="s">
+      <c r="S27" s="6" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="12.75" customHeight="1">
+    <row r="28" spans="1:19" ht="12.75" customHeight="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13" t="s">
         <v>42</v>
@@ -6809,18 +7141,21 @@
         <v>492</v>
       </c>
       <c r="O28" s="1"/>
-      <c r="P28" s="6">
+      <c r="P28" s="65" t="s">
+        <v>677</v>
+      </c>
+      <c r="Q28" s="6">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="Q28" s="6" t="s">
+      <c r="R28" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="R28" s="6" t="s">
+      <c r="S28" s="6" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="12.75" customHeight="1">
+    <row r="29" spans="1:19" ht="12.75" customHeight="1">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -6858,18 +7193,21 @@
         <v>493</v>
       </c>
       <c r="O29" s="1"/>
-      <c r="P29" s="6">
+      <c r="P29" s="65" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q29" s="6">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="R29" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="R29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="12.75" customHeight="1">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13" t="s">
         <v>46</v>
@@ -6907,18 +7245,21 @@
         <v>494</v>
       </c>
       <c r="O30" s="1"/>
-      <c r="P30" s="6">
+      <c r="P30" s="65" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q30" s="6">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="R30" s="6" t="s">
+      <c r="S30" s="6" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="12.75" customHeight="1">
+    <row r="31" spans="1:19" ht="12.75" customHeight="1">
       <c r="A31" s="13" t="s">
         <v>48</v>
       </c>
@@ -6956,18 +7297,21 @@
         <v>495</v>
       </c>
       <c r="O31" s="1"/>
-      <c r="P31" s="6">
+      <c r="P31" s="65" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q31" s="6">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="Q31" s="6" t="s">
+      <c r="R31" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="R31" s="6" t="s">
+      <c r="S31" s="6" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="12.75" customHeight="1">
+    <row r="32" spans="1:19" ht="12.75" customHeight="1">
       <c r="A32" s="13" t="s">
         <v>50</v>
       </c>
@@ -7005,18 +7349,21 @@
         <v>501</v>
       </c>
       <c r="O32" s="1"/>
-      <c r="P32" s="6">
+      <c r="P32" s="65" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q32" s="6">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="Q32" s="6" t="s">
+      <c r="R32" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="R32" s="6" t="s">
+      <c r="S32" s="6" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="12.75" customHeight="1">
+    <row r="33" spans="1:19" ht="12.75" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13" t="s">
         <v>52</v>
@@ -7054,18 +7401,21 @@
         <v>502</v>
       </c>
       <c r="O33" s="1"/>
-      <c r="P33" s="6">
+      <c r="P33" s="65" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q33" s="6">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="Q33" s="6" t="s">
+      <c r="R33" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="R33" s="6" t="s">
+      <c r="S33" s="6" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="12.75" customHeight="1">
+    <row r="34" spans="1:19" ht="12.75" customHeight="1">
       <c r="A34" s="13" t="s">
         <v>54</v>
       </c>
@@ -7103,18 +7453,21 @@
         <v>503</v>
       </c>
       <c r="O34" s="1"/>
-      <c r="P34" s="6">
+      <c r="P34" s="65" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q34" s="6">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="Q34" s="6" t="s">
+      <c r="R34" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="R34" s="6" t="s">
+      <c r="S34" s="6" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="12.75" customHeight="1">
+    <row r="35" spans="1:19" ht="12.75" customHeight="1">
       <c r="A35" s="13"/>
       <c r="B35" s="13" t="s">
         <v>56</v>
@@ -7152,18 +7505,21 @@
         <v>504</v>
       </c>
       <c r="O35" s="1"/>
-      <c r="P35" s="6">
+      <c r="P35" s="65" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q35" s="6">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="Q35" s="6" t="s">
+      <c r="R35" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="R35" s="6" t="s">
+      <c r="S35" s="6" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="12.75" customHeight="1">
+    <row r="36" spans="1:19" ht="12.75" customHeight="1">
       <c r="A36" s="13" t="s">
         <v>58</v>
       </c>
@@ -7201,18 +7557,21 @@
         <v>505</v>
       </c>
       <c r="O36" s="1"/>
-      <c r="P36" s="6">
+      <c r="P36" s="65" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q36" s="6">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="Q36" s="34" t="s">
+      <c r="R36" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="R36" s="6" t="s">
+      <c r="S36" s="6" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="12.75" customHeight="1">
+    <row r="37" spans="1:19" ht="12.75" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
         <v>60</v>
@@ -7248,18 +7607,21 @@
         <v>506</v>
       </c>
       <c r="O37" s="1"/>
-      <c r="P37" s="6">
+      <c r="P37" s="65" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q37" s="6">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="Q37" s="34" t="s">
+      <c r="R37" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="R37" s="6" t="s">
+      <c r="S37" s="6" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="12.75" customHeight="1">
+    <row r="38" spans="1:19" ht="12.75" customHeight="1">
       <c r="A38" s="13" t="s">
         <v>62</v>
       </c>
@@ -7295,18 +7657,21 @@
         <v>507</v>
       </c>
       <c r="O38" s="1"/>
-      <c r="P38" s="6">
+      <c r="P38" s="65" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q38" s="6">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="Q38" s="34" t="s">
+      <c r="R38" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="R38" s="6" t="s">
+      <c r="S38" s="6" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="12.75" customHeight="1">
+    <row r="39" spans="1:19" ht="12.75" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>64</v>
       </c>
@@ -7342,18 +7707,21 @@
         <v>508</v>
       </c>
       <c r="O39" s="40"/>
-      <c r="P39" s="6">
+      <c r="P39" s="66" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q39" s="6">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="Q39" s="34" t="s">
+      <c r="R39" s="34" t="s">
         <v>633</v>
       </c>
-      <c r="R39" s="6" t="s">
+      <c r="S39" s="6" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="12.75" customHeight="1">
+    <row r="40" spans="1:19" ht="12.75" customHeight="1">
       <c r="A40" s="6"/>
       <c r="B40" s="6" t="s">
         <v>65</v>
@@ -7391,18 +7759,21 @@
       <c r="O40" s="35" t="s">
         <v>657</v>
       </c>
-      <c r="P40" s="6">
+      <c r="P40" s="67" t="s">
+        <v>689</v>
+      </c>
+      <c r="Q40" s="6">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="Q40" s="34" t="s">
+      <c r="R40" s="34" t="s">
         <v>372</v>
       </c>
-      <c r="R40" s="6" t="s">
+      <c r="S40" s="6" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="12.75" customHeight="1">
+    <row r="41" spans="1:19" ht="12.75" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>66</v>
       </c>
@@ -7437,18 +7808,21 @@
       <c r="O41" s="35" t="s">
         <v>658</v>
       </c>
-      <c r="P41" s="6">
+      <c r="P41" s="67" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q41" s="6">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="Q41" s="34" t="s">
+      <c r="R41" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="R41" s="6" t="s">
+      <c r="S41" s="6" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="12.75" customHeight="1">
+    <row r="42" spans="1:19" ht="12.75" customHeight="1">
       <c r="A42" s="6"/>
       <c r="B42" s="6" t="s">
         <v>67</v>
@@ -7485,15 +7859,18 @@
       <c r="O42" s="41" t="s">
         <v>659</v>
       </c>
-      <c r="P42" s="6">
+      <c r="P42" s="68" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q42" s="6">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="R42" s="6" t="s">
+      <c r="S42" s="6" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="12.75" customHeight="1">
+    <row r="43" spans="1:19" ht="12.75" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>68</v>
       </c>
@@ -7526,16 +7903,19 @@
       <c r="O43" s="34" t="s">
         <v>660</v>
       </c>
-      <c r="P43" s="6">
+      <c r="P43" s="69" t="s">
+        <v>692</v>
+      </c>
+      <c r="Q43" s="6">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="Q43" s="34"/>
-      <c r="R43" s="6" t="s">
+      <c r="R43" s="34"/>
+      <c r="S43" s="6" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="12.75" customHeight="1">
+    <row r="44" spans="1:19" ht="12.75" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>69</v>
       </c>
@@ -7567,14 +7947,17 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="6">
+      <c r="P44" s="70" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q44" s="6">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
-    </row>
-    <row r="45" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S44" s="6"/>
+    </row>
+    <row r="45" spans="1:19" ht="12.75" customHeight="1">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
         <v>71</v>
@@ -7606,14 +7989,17 @@
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
-      <c r="P45" s="6">
+      <c r="P45" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="Q45" s="6">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
-    </row>
-    <row r="46" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S45" s="6"/>
+    </row>
+    <row r="46" spans="1:19" ht="12.75" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>73</v>
       </c>
@@ -7645,14 +8031,17 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
-      <c r="P46" s="6">
+      <c r="P46" s="70" t="s">
+        <v>695</v>
+      </c>
+      <c r="Q46" s="6">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
-    </row>
-    <row r="47" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S46" s="6"/>
+    </row>
+    <row r="47" spans="1:19" ht="12.75" customHeight="1">
       <c r="A47" s="6"/>
       <c r="B47" s="6" t="s">
         <v>75</v>
@@ -7684,14 +8073,17 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
-      <c r="P47" s="6">
+      <c r="P47" s="70" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q47" s="6">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
-    </row>
-    <row r="48" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S47" s="6"/>
+    </row>
+    <row r="48" spans="1:19" ht="12.75" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>77</v>
       </c>
@@ -7723,14 +8115,17 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
-      <c r="P48" s="6">
+      <c r="P48" s="70" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q48" s="6">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
-    </row>
-    <row r="49" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S48" s="6"/>
+    </row>
+    <row r="49" spans="1:19" ht="12.75" customHeight="1">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
         <v>79</v>
@@ -7764,14 +8159,17 @@
       </c>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
-      <c r="P49" s="6">
+      <c r="P49" s="70" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q49" s="6">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="Q49" s="6"/>
       <c r="R49" s="6"/>
-    </row>
-    <row r="50" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="1:19" ht="12.75" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>81</v>
       </c>
@@ -7801,14 +8199,17 @@
       </c>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
-      <c r="P50" s="6">
+      <c r="P50" s="70" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q50" s="6">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
-    </row>
-    <row r="51" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S50" s="6"/>
+    </row>
+    <row r="51" spans="1:19" ht="12.75" customHeight="1">
       <c r="A51" s="13" t="s">
         <v>83</v>
       </c>
@@ -7840,14 +8241,17 @@
       </c>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
-      <c r="P51" s="6">
+      <c r="P51" s="70" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q51" s="6">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="Q51" s="6"/>
       <c r="R51" s="6"/>
-    </row>
-    <row r="52" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S51" s="6"/>
+    </row>
+    <row r="52" spans="1:19" ht="12.75" customHeight="1">
       <c r="A52" s="13"/>
       <c r="B52" s="13" t="s">
         <v>85</v>
@@ -7880,14 +8284,17 @@
       </c>
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
-      <c r="P52" s="6">
+      <c r="P52" s="70" t="s">
+        <v>701</v>
+      </c>
+      <c r="Q52" s="6">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
-    </row>
-    <row r="53" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S52" s="6"/>
+    </row>
+    <row r="53" spans="1:19" ht="12.75" customHeight="1">
       <c r="A53" s="13" t="s">
         <v>87</v>
       </c>
@@ -7920,14 +8327,17 @@
       </c>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
-      <c r="P53" s="6">
+      <c r="P53" s="70" t="s">
+        <v>702</v>
+      </c>
+      <c r="Q53" s="6">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
-    </row>
-    <row r="54" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" ht="12.75" customHeight="1">
       <c r="A54" s="13"/>
       <c r="B54" s="13" t="s">
         <v>88</v>
@@ -7960,14 +8370,17 @@
       </c>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
-      <c r="P54" s="6">
+      <c r="P54" s="70" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q54" s="6">
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
-    </row>
-    <row r="55" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S54" s="6"/>
+    </row>
+    <row r="55" spans="1:19" ht="12.75" customHeight="1">
       <c r="A55" s="13" t="s">
         <v>89</v>
       </c>
@@ -8000,14 +8413,17 @@
       </c>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
-      <c r="P55" s="6">
+      <c r="P55" s="70" t="s">
+        <v>704</v>
+      </c>
+      <c r="Q55" s="6">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
-    </row>
-    <row r="56" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S55" s="6"/>
+    </row>
+    <row r="56" spans="1:19" ht="12.75" customHeight="1">
       <c r="A56" s="13" t="s">
         <v>90</v>
       </c>
@@ -8040,14 +8456,17 @@
       </c>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
-      <c r="P56" s="6">
+      <c r="P56" s="70" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q56" s="6">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="Q56" s="6"/>
       <c r="R56" s="6"/>
-    </row>
-    <row r="57" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S56" s="6"/>
+    </row>
+    <row r="57" spans="1:19" ht="12.75" customHeight="1">
       <c r="A57" s="13"/>
       <c r="B57" s="13" t="s">
         <v>91</v>
@@ -8078,14 +8497,17 @@
       </c>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
-      <c r="P57" s="6">
+      <c r="P57" s="70" t="s">
+        <v>706</v>
+      </c>
+      <c r="Q57" s="6">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
-    </row>
-    <row r="58" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S57" s="6"/>
+    </row>
+    <row r="58" spans="1:19" ht="12.75" customHeight="1">
       <c r="A58" s="13" t="s">
         <v>92</v>
       </c>
@@ -8114,14 +8536,17 @@
       </c>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
-      <c r="P58" s="6">
+      <c r="P58" s="70" t="s">
+        <v>707</v>
+      </c>
+      <c r="Q58" s="6">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="Q58" s="6"/>
       <c r="R58" s="6"/>
-    </row>
-    <row r="59" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S58" s="6"/>
+    </row>
+    <row r="59" spans="1:19" ht="12.75" customHeight="1">
       <c r="A59" s="13"/>
       <c r="B59" s="13" t="s">
         <v>93</v>
@@ -8150,14 +8575,17 @@
       </c>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
-      <c r="P59" s="6">
+      <c r="P59" s="70" t="s">
+        <v>708</v>
+      </c>
+      <c r="Q59" s="6">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="Q59" s="6"/>
       <c r="R59" s="6"/>
-    </row>
-    <row r="60" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S59" s="6"/>
+    </row>
+    <row r="60" spans="1:19" ht="12.75" customHeight="1">
       <c r="A60" s="13" t="s">
         <v>94</v>
       </c>
@@ -8186,14 +8614,17 @@
       </c>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
-      <c r="P60" s="6">
+      <c r="P60" s="70" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q60" s="6">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="Q60" s="6"/>
       <c r="R60" s="6"/>
-    </row>
-    <row r="61" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S60" s="6"/>
+    </row>
+    <row r="61" spans="1:19" ht="12.75" customHeight="1">
       <c r="A61" s="13"/>
       <c r="B61" s="13" t="s">
         <v>95</v>
@@ -8222,14 +8653,17 @@
       </c>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
-      <c r="P61" s="6">
+      <c r="P61" s="70" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q61" s="6">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="Q61" s="6"/>
       <c r="R61" s="6"/>
-    </row>
-    <row r="62" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S61" s="6"/>
+    </row>
+    <row r="62" spans="1:19" ht="12.75" customHeight="1">
       <c r="A62" s="13" t="s">
         <v>96</v>
       </c>
@@ -8258,14 +8692,17 @@
       </c>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
-      <c r="P62" s="6">
+      <c r="P62" s="70" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q62" s="6">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
-    </row>
-    <row r="63" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S62" s="6"/>
+    </row>
+    <row r="63" spans="1:19" ht="12.75" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>97</v>
       </c>
@@ -8294,14 +8731,17 @@
       </c>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
-      <c r="P63" s="6">
+      <c r="P63" s="70" t="s">
+        <v>712</v>
+      </c>
+      <c r="Q63" s="6">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
-    </row>
-    <row r="64" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S63" s="6"/>
+    </row>
+    <row r="64" spans="1:19" ht="12.75" customHeight="1">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
         <v>98</v>
@@ -8330,14 +8770,17 @@
       </c>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
-      <c r="P64" s="6">
+      <c r="P64" s="70" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q64" s="6">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
-    </row>
-    <row r="65" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S64" s="6"/>
+    </row>
+    <row r="65" spans="1:19" ht="12.75" customHeight="1">
       <c r="A65" s="6" t="s">
         <v>99</v>
       </c>
@@ -8366,14 +8809,17 @@
       </c>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
-      <c r="P65" s="6">
+      <c r="P65" s="70" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q65" s="6">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
-    </row>
-    <row r="66" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S65" s="6"/>
+    </row>
+    <row r="66" spans="1:19" ht="12.75" customHeight="1">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
         <v>100</v>
@@ -8402,14 +8848,17 @@
       </c>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
-      <c r="P66" s="6">
+      <c r="P66" s="70" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q66" s="6">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="Q66" s="6"/>
       <c r="R66" s="6"/>
-    </row>
-    <row r="67" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S66" s="6"/>
+    </row>
+    <row r="67" spans="1:19" ht="12.75" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>101</v>
       </c>
@@ -8438,14 +8887,17 @@
       </c>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
-      <c r="P67" s="6">
+      <c r="P67" s="70" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q67" s="6">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="Q67" s="6"/>
       <c r="R67" s="6"/>
-    </row>
-    <row r="68" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S67" s="6"/>
+    </row>
+    <row r="68" spans="1:19" ht="12.75" customHeight="1">
       <c r="A68" s="6" t="s">
         <v>102</v>
       </c>
@@ -8474,14 +8926,17 @@
       </c>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
-      <c r="P68" s="6">
-        <f t="shared" ref="P68:P86" si="3">P67+1</f>
+      <c r="P68" s="70" t="s">
+        <v>717</v>
+      </c>
+      <c r="Q68" s="6">
+        <f t="shared" ref="Q68:Q86" si="3">Q67+1</f>
         <v>101</v>
       </c>
-      <c r="Q68" s="6"/>
       <c r="R68" s="6"/>
-    </row>
-    <row r="69" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S68" s="6"/>
+    </row>
+    <row r="69" spans="1:19" ht="12.75" customHeight="1">
       <c r="A69" s="6"/>
       <c r="B69" s="6" t="s">
         <v>103</v>
@@ -8506,14 +8961,17 @@
       </c>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
-      <c r="P69" s="6">
+      <c r="P69" s="70" t="s">
+        <v>718</v>
+      </c>
+      <c r="Q69" s="6">
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="Q69" s="6"/>
       <c r="R69" s="6"/>
-    </row>
-    <row r="70" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S69" s="6"/>
+    </row>
+    <row r="70" spans="1:19" ht="12.75" customHeight="1">
       <c r="A70" s="6" t="s">
         <v>104</v>
       </c>
@@ -8542,14 +9000,17 @@
       </c>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
-      <c r="P70" s="6">
+      <c r="P70" s="70" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q70" s="6">
         <f t="shared" si="3"/>
         <v>103</v>
       </c>
-      <c r="Q70" s="6"/>
       <c r="R70" s="6"/>
-    </row>
-    <row r="71" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S70" s="6"/>
+    </row>
+    <row r="71" spans="1:19" ht="12.75" customHeight="1">
       <c r="A71" s="6"/>
       <c r="B71" s="6" t="s">
         <v>105</v>
@@ -8574,14 +9035,17 @@
       </c>
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
-      <c r="P71" s="6">
+      <c r="P71" s="70" t="s">
+        <v>720</v>
+      </c>
+      <c r="Q71" s="6">
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="Q71" s="6"/>
       <c r="R71" s="6"/>
-    </row>
-    <row r="72" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S71" s="6"/>
+    </row>
+    <row r="72" spans="1:19" ht="12.75" customHeight="1">
       <c r="A72" s="6" t="s">
         <v>106</v>
       </c>
@@ -8606,14 +9070,15 @@
       </c>
       <c r="N72" s="6"/>
       <c r="O72" s="6"/>
-      <c r="P72" s="6">
+      <c r="P72" s="6"/>
+      <c r="Q72" s="6">
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="Q72" s="6"/>
       <c r="R72" s="6"/>
-    </row>
-    <row r="73" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S72" s="6"/>
+    </row>
+    <row r="73" spans="1:19" ht="12.75" customHeight="1">
       <c r="A73" s="6"/>
       <c r="B73" s="6" t="s">
         <v>107</v>
@@ -8638,14 +9103,15 @@
       </c>
       <c r="N73" s="6"/>
       <c r="O73" s="6"/>
-      <c r="P73" s="6">
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6">
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
-      <c r="Q73" s="6"/>
       <c r="R73" s="6"/>
-    </row>
-    <row r="74" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S73" s="6"/>
+    </row>
+    <row r="74" spans="1:19" ht="12.75" customHeight="1">
       <c r="A74" s="6" t="s">
         <v>108</v>
       </c>
@@ -8670,14 +9136,15 @@
       </c>
       <c r="N74" s="6"/>
       <c r="O74" s="6"/>
-      <c r="P74" s="6">
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6">
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
-      <c r="Q74" s="6"/>
       <c r="R74" s="6"/>
-    </row>
-    <row r="75" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S74" s="6"/>
+    </row>
+    <row r="75" spans="1:19" ht="12.75" customHeight="1">
       <c r="A75" s="30" t="s">
         <v>109</v>
       </c>
@@ -8702,14 +9169,15 @@
       </c>
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
-      <c r="P75" s="6">
+      <c r="P75" s="6"/>
+      <c r="Q75" s="6">
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
-      <c r="Q75" s="6"/>
       <c r="R75" s="6"/>
-    </row>
-    <row r="76" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S75" s="6"/>
+    </row>
+    <row r="76" spans="1:19" ht="12.75" customHeight="1">
       <c r="A76" s="13"/>
       <c r="B76" s="13" t="s">
         <v>110</v>
@@ -8734,14 +9202,15 @@
       </c>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
-      <c r="P76" s="6">
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6">
         <f t="shared" si="3"/>
         <v>109</v>
       </c>
-      <c r="Q76" s="6"/>
       <c r="R76" s="6"/>
-    </row>
-    <row r="77" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S76" s="6"/>
+    </row>
+    <row r="77" spans="1:19" ht="12.75" customHeight="1">
       <c r="A77" s="13" t="s">
         <v>111</v>
       </c>
@@ -8766,14 +9235,15 @@
       </c>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
-      <c r="P77" s="6">
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="Q77" s="6"/>
       <c r="R77" s="6"/>
-    </row>
-    <row r="78" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S77" s="6"/>
+    </row>
+    <row r="78" spans="1:19" ht="12.75" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="13" t="s">
         <v>112</v>
@@ -8798,14 +9268,15 @@
       </c>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
-      <c r="P78" s="6">
+      <c r="P78" s="6"/>
+      <c r="Q78" s="6">
         <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="Q78" s="6"/>
       <c r="R78" s="6"/>
-    </row>
-    <row r="79" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S78" s="6"/>
+    </row>
+    <row r="79" spans="1:19" ht="12.75" customHeight="1">
       <c r="A79" s="13" t="s">
         <v>113</v>
       </c>
@@ -8830,14 +9301,15 @@
       </c>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
-      <c r="P79" s="6">
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6">
         <f t="shared" si="3"/>
         <v>112</v>
       </c>
-      <c r="Q79" s="6"/>
       <c r="R79" s="6"/>
-    </row>
-    <row r="80" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S79" s="6"/>
+    </row>
+    <row r="80" spans="1:19" ht="12.75" customHeight="1">
       <c r="A80" s="13" t="s">
         <v>114</v>
       </c>
@@ -8862,14 +9334,15 @@
       </c>
       <c r="N80" s="6"/>
       <c r="O80" s="6"/>
-      <c r="P80" s="6">
+      <c r="P80" s="6"/>
+      <c r="Q80" s="6">
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="Q80" s="6"/>
       <c r="R80" s="6"/>
-    </row>
-    <row r="81" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S80" s="6"/>
+    </row>
+    <row r="81" spans="1:19" ht="12.75" customHeight="1">
       <c r="A81" s="13"/>
       <c r="B81" s="13" t="s">
         <v>115</v>
@@ -8894,14 +9367,15 @@
       </c>
       <c r="N81" s="6"/>
       <c r="O81" s="6"/>
-      <c r="P81" s="6">
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
-      <c r="Q81" s="6"/>
       <c r="R81" s="6"/>
-    </row>
-    <row r="82" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S81" s="6"/>
+    </row>
+    <row r="82" spans="1:19" ht="12.75" customHeight="1">
       <c r="A82" s="13" t="s">
         <v>116</v>
       </c>
@@ -8926,14 +9400,15 @@
       </c>
       <c r="N82" s="6"/>
       <c r="O82" s="6"/>
-      <c r="P82" s="6">
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6">
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
-      <c r="Q82" s="6"/>
       <c r="R82" s="6"/>
-    </row>
-    <row r="83" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S82" s="6"/>
+    </row>
+    <row r="83" spans="1:19" ht="12.75" customHeight="1">
       <c r="A83" s="13"/>
       <c r="B83" s="13" t="s">
         <v>117</v>
@@ -8958,14 +9433,15 @@
       </c>
       <c r="N83" s="6"/>
       <c r="O83" s="6"/>
-      <c r="P83" s="6">
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6">
         <f t="shared" si="3"/>
         <v>116</v>
       </c>
-      <c r="Q83" s="6"/>
       <c r="R83" s="6"/>
-    </row>
-    <row r="84" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S83" s="6"/>
+    </row>
+    <row r="84" spans="1:19" ht="12.75" customHeight="1">
       <c r="A84" s="13" t="s">
         <v>118</v>
       </c>
@@ -8990,14 +9466,15 @@
       </c>
       <c r="N84" s="6"/>
       <c r="O84" s="6"/>
-      <c r="P84" s="6">
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6">
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
-      <c r="Q84" s="6"/>
       <c r="R84" s="6"/>
-    </row>
-    <row r="85" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S84" s="6"/>
+    </row>
+    <row r="85" spans="1:19" ht="12.75" customHeight="1">
       <c r="A85" s="13"/>
       <c r="B85" s="13" t="s">
         <v>119</v>
@@ -9022,14 +9499,15 @@
       </c>
       <c r="N85" s="6"/>
       <c r="O85" s="6"/>
-      <c r="P85" s="6">
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6">
         <f t="shared" si="3"/>
         <v>118</v>
       </c>
-      <c r="Q85" s="6"/>
       <c r="R85" s="6"/>
-    </row>
-    <row r="86" spans="1:18" ht="12.75" customHeight="1">
+      <c r="S85" s="6"/>
+    </row>
+    <row r="86" spans="1:19" ht="12.75" customHeight="1">
       <c r="A86" s="13" t="s">
         <v>120</v>
       </c>
@@ -9054,11 +9532,12 @@
       </c>
       <c r="N86" s="6"/>
       <c r="O86" s="6"/>
-      <c r="P86" s="6">
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6">
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
-      <c r="R86" s="6"/>
+      <c r="S86" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
加 OrganBike excel table
</commit_message>
<xml_diff>
--- a/MPC82/PitchTable.xlsx
+++ b/MPC82/PitchTable.xlsx
@@ -4838,135 +4838,135 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>25(P00)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>26(P01)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>27(P02)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>28(P03)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>29(P04)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>30(P05)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>31(P06)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>32(P07)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>33(P11)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>34(P14)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>35(P15)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>36(P16)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>37(P17)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>38(P20)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>39(P21)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>40(P22)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>41(P23)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>42(P24)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>43(P25)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>44(P26)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>45(P56)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>46(P55)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>47(P34)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>48(P35)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>49(P36)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>50(P37)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>51(P40)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>52(P41)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>53(P42)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>54(P43)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>55(P46)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>56(P50)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>57(P51)</t>
+    <t>1(P00)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2(P01)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3(P02)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(P03)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5(P04)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>6(P05)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>7(P06)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8(P07)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9(P11)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10(P14)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>11(P15)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>12(P16)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>13(P17)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14(P20)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>15(P21)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>16(P22)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>17(P23)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>18(P24)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>19(P25)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20(P26)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>21(P56)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>22(P55)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>23(P34)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>24(P35)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>25(P36)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>26(P37)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>29(P40)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>30(P41)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>31(P42)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>32(P43)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>33(P46)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>34(P50)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>35(P51)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -5022,7 +5022,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5140,6 +5140,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA26D2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5335,7 +5371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5489,30 +5525,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5549,12 +5561,60 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA26D2"/>
+      <color rgb="FFFF9900"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -5846,10 +5906,10 @@
   <dimension ref="A1:S86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P72" sqref="P72"/>
+      <selection pane="bottomRight" activeCell="P71" sqref="P71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -5917,10 +5977,10 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="63"/>
       <c r="C2" s="17">
         <v>0</v>
       </c>
@@ -5958,7 +6018,7 @@
         <v>9</v>
       </c>
       <c r="O2" s="6"/>
-      <c r="P2" s="62"/>
+      <c r="P2" s="54"/>
       <c r="Q2" s="14">
         <v>35</v>
       </c>
@@ -5995,7 +6055,7 @@
         <v>473</v>
       </c>
       <c r="O3" s="16"/>
-      <c r="P3" s="59"/>
+      <c r="P3" s="51"/>
       <c r="Q3" s="6">
         <f>Q2+1</f>
         <v>36</v>
@@ -6052,7 +6112,7 @@
       <c r="O4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="59">
+      <c r="P4" s="51">
         <v>6</v>
       </c>
       <c r="Q4" s="6">
@@ -6097,7 +6157,7 @@
         <v>475</v>
       </c>
       <c r="O5" s="16"/>
-      <c r="P5" s="59"/>
+      <c r="P5" s="51"/>
       <c r="Q5" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -6140,7 +6200,7 @@
         <v>476</v>
       </c>
       <c r="O6" s="16"/>
-      <c r="P6" s="59"/>
+      <c r="P6" s="51"/>
       <c r="Q6" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -6185,7 +6245,7 @@
         <v>477</v>
       </c>
       <c r="O7" s="16"/>
-      <c r="P7" s="59"/>
+      <c r="P7" s="51"/>
       <c r="Q7" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -6230,7 +6290,7 @@
         <v>478</v>
       </c>
       <c r="O8" s="16"/>
-      <c r="P8" s="59"/>
+      <c r="P8" s="51"/>
       <c r="Q8" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -6275,7 +6335,7 @@
         <v>479</v>
       </c>
       <c r="O9" s="16"/>
-      <c r="P9" s="59"/>
+      <c r="P9" s="51"/>
       <c r="Q9" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -6320,7 +6380,7 @@
         <v>480</v>
       </c>
       <c r="O10" s="16"/>
-      <c r="P10" s="59"/>
+      <c r="P10" s="51"/>
       <c r="Q10" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -6365,7 +6425,7 @@
         <v>481</v>
       </c>
       <c r="O11" s="16"/>
-      <c r="P11" s="59"/>
+      <c r="P11" s="51"/>
       <c r="Q11" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -6410,7 +6470,7 @@
         <v>653</v>
       </c>
       <c r="O12" s="24"/>
-      <c r="P12" s="59"/>
+      <c r="P12" s="51"/>
       <c r="Q12" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6454,10 +6514,10 @@
       <c r="N13" s="31" t="s">
         <v>482</v>
       </c>
-      <c r="O13" s="52" t="s">
+      <c r="O13" s="64" t="s">
         <v>654</v>
       </c>
-      <c r="P13" s="60"/>
+      <c r="P13" s="52"/>
       <c r="Q13" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -6501,8 +6561,8 @@
       <c r="N14" s="33" t="s">
         <v>483</v>
       </c>
-      <c r="O14" s="53"/>
-      <c r="P14" s="61"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="53"/>
       <c r="Q14" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -6540,8 +6600,8 @@
       <c r="N15" s="31" t="s">
         <v>484</v>
       </c>
-      <c r="O15" s="53"/>
-      <c r="P15" s="63" t="s">
+      <c r="O15" s="65"/>
+      <c r="P15" s="55" t="s">
         <v>664</v>
       </c>
       <c r="Q15" s="6">
@@ -6578,8 +6638,8 @@
       <c r="N16" s="33" t="s">
         <v>485</v>
       </c>
-      <c r="O16" s="54"/>
-      <c r="P16" s="63" t="s">
+      <c r="O16" s="66"/>
+      <c r="P16" s="55" t="s">
         <v>665</v>
       </c>
       <c r="Q16" s="6">
@@ -6620,7 +6680,7 @@
         <v>486</v>
       </c>
       <c r="O17" s="7"/>
-      <c r="P17" s="64" t="s">
+      <c r="P17" s="56" t="s">
         <v>666</v>
       </c>
       <c r="Q17" s="6">
@@ -6659,7 +6719,7 @@
         <v>487</v>
       </c>
       <c r="O18" s="16"/>
-      <c r="P18" s="64" t="s">
+      <c r="P18" s="56" t="s">
         <v>667</v>
       </c>
       <c r="Q18" s="6">
@@ -6702,7 +6762,7 @@
         <v>488</v>
       </c>
       <c r="O19" s="16"/>
-      <c r="P19" s="64" t="s">
+      <c r="P19" s="56" t="s">
         <v>668</v>
       </c>
       <c r="Q19" s="6">
@@ -6749,7 +6809,7 @@
         <v>489</v>
       </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="65" t="s">
+      <c r="P20" s="57" t="s">
         <v>669</v>
       </c>
       <c r="Q20" s="6">
@@ -6796,7 +6856,7 @@
         <v>490</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="65" t="s">
+      <c r="P21" s="57" t="s">
         <v>670</v>
       </c>
       <c r="Q21" s="6">
@@ -6843,7 +6903,7 @@
         <v>496</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="65" t="s">
+      <c r="P22" s="57" t="s">
         <v>671</v>
       </c>
       <c r="Q22" s="6">
@@ -6890,7 +6950,7 @@
         <v>498</v>
       </c>
       <c r="O23" s="1"/>
-      <c r="P23" s="65" t="s">
+      <c r="P23" s="57" t="s">
         <v>672</v>
       </c>
       <c r="Q23" s="6">
@@ -6939,7 +6999,7 @@
         <v>497</v>
       </c>
       <c r="O24" s="40"/>
-      <c r="P24" s="66" t="s">
+      <c r="P24" s="58" t="s">
         <v>673</v>
       </c>
       <c r="Q24" s="6">
@@ -6988,7 +7048,7 @@
         <v>499</v>
       </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="65" t="s">
+      <c r="P25" s="57" t="s">
         <v>674</v>
       </c>
       <c r="Q25" s="6">
@@ -7037,7 +7097,7 @@
         <v>500</v>
       </c>
       <c r="O26" s="1"/>
-      <c r="P26" s="65" t="s">
+      <c r="P26" s="57" t="s">
         <v>675</v>
       </c>
       <c r="Q26" s="6">
@@ -7089,7 +7149,7 @@
         <v>491</v>
       </c>
       <c r="O27" s="1"/>
-      <c r="P27" s="65" t="s">
+      <c r="P27" s="57" t="s">
         <v>676</v>
       </c>
       <c r="Q27" s="6">
@@ -7141,7 +7201,7 @@
         <v>492</v>
       </c>
       <c r="O28" s="1"/>
-      <c r="P28" s="65" t="s">
+      <c r="P28" s="57" t="s">
         <v>677</v>
       </c>
       <c r="Q28" s="6">
@@ -7193,7 +7253,7 @@
         <v>493</v>
       </c>
       <c r="O29" s="1"/>
-      <c r="P29" s="65" t="s">
+      <c r="P29" s="57" t="s">
         <v>678</v>
       </c>
       <c r="Q29" s="6">
@@ -7245,7 +7305,7 @@
         <v>494</v>
       </c>
       <c r="O30" s="1"/>
-      <c r="P30" s="65" t="s">
+      <c r="P30" s="57" t="s">
         <v>679</v>
       </c>
       <c r="Q30" s="6">
@@ -7297,7 +7357,7 @@
         <v>495</v>
       </c>
       <c r="O31" s="1"/>
-      <c r="P31" s="65" t="s">
+      <c r="P31" s="57" t="s">
         <v>680</v>
       </c>
       <c r="Q31" s="6">
@@ -7349,7 +7409,7 @@
         <v>501</v>
       </c>
       <c r="O32" s="1"/>
-      <c r="P32" s="65" t="s">
+      <c r="P32" s="57" t="s">
         <v>681</v>
       </c>
       <c r="Q32" s="6">
@@ -7401,7 +7461,7 @@
         <v>502</v>
       </c>
       <c r="O33" s="1"/>
-      <c r="P33" s="65" t="s">
+      <c r="P33" s="57" t="s">
         <v>682</v>
       </c>
       <c r="Q33" s="6">
@@ -7453,7 +7513,7 @@
         <v>503</v>
       </c>
       <c r="O34" s="1"/>
-      <c r="P34" s="65" t="s">
+      <c r="P34" s="57" t="s">
         <v>683</v>
       </c>
       <c r="Q34" s="6">
@@ -7505,7 +7565,7 @@
         <v>504</v>
       </c>
       <c r="O35" s="1"/>
-      <c r="P35" s="65" t="s">
+      <c r="P35" s="57" t="s">
         <v>684</v>
       </c>
       <c r="Q35" s="6">
@@ -7557,7 +7617,7 @@
         <v>505</v>
       </c>
       <c r="O36" s="1"/>
-      <c r="P36" s="65" t="s">
+      <c r="P36" s="57" t="s">
         <v>685</v>
       </c>
       <c r="Q36" s="6">
@@ -7607,7 +7667,7 @@
         <v>506</v>
       </c>
       <c r="O37" s="1"/>
-      <c r="P37" s="65" t="s">
+      <c r="P37" s="57" t="s">
         <v>686</v>
       </c>
       <c r="Q37" s="6">
@@ -7657,7 +7717,7 @@
         <v>507</v>
       </c>
       <c r="O38" s="1"/>
-      <c r="P38" s="65" t="s">
+      <c r="P38" s="57" t="s">
         <v>687</v>
       </c>
       <c r="Q38" s="6">
@@ -7707,7 +7767,7 @@
         <v>508</v>
       </c>
       <c r="O39" s="40"/>
-      <c r="P39" s="66" t="s">
+      <c r="P39" s="58" t="s">
         <v>688</v>
       </c>
       <c r="Q39" s="6">
@@ -7759,7 +7819,7 @@
       <c r="O40" s="35" t="s">
         <v>657</v>
       </c>
-      <c r="P40" s="67" t="s">
+      <c r="P40" s="59" t="s">
         <v>689</v>
       </c>
       <c r="Q40" s="6">
@@ -7808,7 +7868,7 @@
       <c r="O41" s="35" t="s">
         <v>658</v>
       </c>
-      <c r="P41" s="67" t="s">
+      <c r="P41" s="59" t="s">
         <v>690</v>
       </c>
       <c r="Q41" s="6">
@@ -7859,7 +7919,7 @@
       <c r="O42" s="41" t="s">
         <v>659</v>
       </c>
-      <c r="P42" s="68" t="s">
+      <c r="P42" s="60" t="s">
         <v>691</v>
       </c>
       <c r="Q42" s="6">
@@ -7903,7 +7963,7 @@
       <c r="O43" s="34" t="s">
         <v>660</v>
       </c>
-      <c r="P43" s="69" t="s">
+      <c r="P43" s="61" t="s">
         <v>692</v>
       </c>
       <c r="Q43" s="6">
@@ -7947,7 +8007,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="70" t="s">
+      <c r="P44" s="62" t="s">
         <v>693</v>
       </c>
       <c r="Q44" s="6">
@@ -7989,7 +8049,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
-      <c r="P45" s="70" t="s">
+      <c r="P45" s="62" t="s">
         <v>694</v>
       </c>
       <c r="Q45" s="6">
@@ -8031,7 +8091,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
-      <c r="P46" s="70" t="s">
+      <c r="P46" s="62" t="s">
         <v>695</v>
       </c>
       <c r="Q46" s="6">
@@ -8073,7 +8133,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
-      <c r="P47" s="70" t="s">
+      <c r="P47" s="62" t="s">
         <v>696</v>
       </c>
       <c r="Q47" s="6">
@@ -8115,7 +8175,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
-      <c r="P48" s="70" t="s">
+      <c r="P48" s="62" t="s">
         <v>697</v>
       </c>
       <c r="Q48" s="6">
@@ -8159,7 +8219,7 @@
       </c>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
-      <c r="P49" s="70" t="s">
+      <c r="P49" s="62" t="s">
         <v>698</v>
       </c>
       <c r="Q49" s="6">
@@ -8199,7 +8259,7 @@
       </c>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
-      <c r="P50" s="70" t="s">
+      <c r="P50" s="62" t="s">
         <v>699</v>
       </c>
       <c r="Q50" s="6">
@@ -8241,7 +8301,7 @@
       </c>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
-      <c r="P51" s="70" t="s">
+      <c r="P51" s="62" t="s">
         <v>700</v>
       </c>
       <c r="Q51" s="6">
@@ -8284,7 +8344,7 @@
       </c>
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
-      <c r="P52" s="70" t="s">
+      <c r="P52" s="62" t="s">
         <v>701</v>
       </c>
       <c r="Q52" s="6">
@@ -8327,7 +8387,7 @@
       </c>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
-      <c r="P53" s="70" t="s">
+      <c r="P53" s="62" t="s">
         <v>702</v>
       </c>
       <c r="Q53" s="6">
@@ -8370,7 +8430,7 @@
       </c>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
-      <c r="P54" s="70" t="s">
+      <c r="P54" s="62" t="s">
         <v>703</v>
       </c>
       <c r="Q54" s="6">
@@ -8413,7 +8473,7 @@
       </c>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
-      <c r="P55" s="70" t="s">
+      <c r="P55" s="62" t="s">
         <v>704</v>
       </c>
       <c r="Q55" s="6">
@@ -8456,7 +8516,7 @@
       </c>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
-      <c r="P56" s="70" t="s">
+      <c r="P56" s="62" t="s">
         <v>705</v>
       </c>
       <c r="Q56" s="6">
@@ -8497,7 +8557,7 @@
       </c>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
-      <c r="P57" s="70" t="s">
+      <c r="P57" s="62" t="s">
         <v>706</v>
       </c>
       <c r="Q57" s="6">
@@ -8536,7 +8596,7 @@
       </c>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
-      <c r="P58" s="70" t="s">
+      <c r="P58" s="62" t="s">
         <v>707</v>
       </c>
       <c r="Q58" s="6">
@@ -8575,7 +8635,7 @@
       </c>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
-      <c r="P59" s="70" t="s">
+      <c r="P59" s="62" t="s">
         <v>708</v>
       </c>
       <c r="Q59" s="6">
@@ -8614,7 +8674,7 @@
       </c>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
-      <c r="P60" s="70" t="s">
+      <c r="P60" s="62" t="s">
         <v>709</v>
       </c>
       <c r="Q60" s="6">
@@ -8653,7 +8713,7 @@
       </c>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
-      <c r="P61" s="70" t="s">
+      <c r="P61" s="62" t="s">
         <v>710</v>
       </c>
       <c r="Q61" s="6">
@@ -8692,7 +8752,7 @@
       </c>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
-      <c r="P62" s="70" t="s">
+      <c r="P62" s="62" t="s">
         <v>711</v>
       </c>
       <c r="Q62" s="6">
@@ -8731,7 +8791,7 @@
       </c>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
-      <c r="P63" s="70" t="s">
+      <c r="P63" s="71" t="s">
         <v>712</v>
       </c>
       <c r="Q63" s="6">
@@ -8770,7 +8830,7 @@
       </c>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
-      <c r="P64" s="70" t="s">
+      <c r="P64" s="3" t="s">
         <v>713</v>
       </c>
       <c r="Q64" s="6">
@@ -8809,7 +8869,7 @@
       </c>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
-      <c r="P65" s="70" t="s">
+      <c r="P65" s="13" t="s">
         <v>714</v>
       </c>
       <c r="Q65" s="6">
@@ -8848,7 +8908,7 @@
       </c>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
-      <c r="P66" s="70" t="s">
+      <c r="P66" s="72" t="s">
         <v>715</v>
       </c>
       <c r="Q66" s="6">
@@ -8887,7 +8947,7 @@
       </c>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
-      <c r="P67" s="70" t="s">
+      <c r="P67" s="73" t="s">
         <v>716</v>
       </c>
       <c r="Q67" s="6">
@@ -8926,7 +8986,7 @@
       </c>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
-      <c r="P68" s="70" t="s">
+      <c r="P68" s="74" t="s">
         <v>717</v>
       </c>
       <c r="Q68" s="6">
@@ -8961,7 +9021,7 @@
       </c>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
-      <c r="P69" s="70" t="s">
+      <c r="P69" s="76" t="s">
         <v>718</v>
       </c>
       <c r="Q69" s="6">
@@ -9000,7 +9060,7 @@
       </c>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
-      <c r="P70" s="70" t="s">
+      <c r="P70" s="62" t="s">
         <v>719</v>
       </c>
       <c r="Q70" s="6">
@@ -9035,7 +9095,7 @@
       </c>
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
-      <c r="P71" s="70" t="s">
+      <c r="P71" s="75" t="s">
         <v>720</v>
       </c>
       <c r="Q71" s="6">
@@ -10386,7 +10446,7 @@
       <c r="N24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O24" s="55" t="s">
+      <c r="O24" s="67" t="s">
         <v>37</v>
       </c>
       <c r="P24" s="16"/>
@@ -10423,7 +10483,7 @@
       <c r="N25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="O25" s="53"/>
+      <c r="O25" s="65"/>
       <c r="P25" s="16"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
@@ -10458,7 +10518,7 @@
       <c r="N26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O26" s="53"/>
+      <c r="O26" s="65"/>
       <c r="P26" s="16"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
@@ -10493,7 +10553,7 @@
       <c r="N27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="O27" s="54"/>
+      <c r="O27" s="66"/>
       <c r="P27" s="16"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
@@ -13510,11 +13570,11 @@
       <c r="C20" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="68" t="s">
         <v>185</v>
       </c>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="9" t="s">
         <v>186</v>
       </c>
@@ -13564,11 +13624,11 @@
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="68" t="s">
         <v>187</v>
       </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -13624,20 +13684,20 @@
       <c r="A25" s="6">
         <v>8</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="69" t="s">
         <v>188</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -13826,20 +13886,20 @@
       <c r="A35" s="6">
         <v>18</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
@@ -15443,7 +15503,7 @@
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1">
       <c r="A11" s="19"/>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="70" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -15484,7 +15544,7 @@
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1">
       <c r="A12" s="19"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="19" t="s">
         <v>220</v>
       </c>
@@ -15523,7 +15583,7 @@
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1">
       <c r="A13" s="19"/>
-      <c r="B13" s="58"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="19" t="s">
         <v>223</v>
       </c>
@@ -15562,7 +15622,7 @@
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1">
       <c r="A14" s="19"/>
-      <c r="B14" s="58"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="19" t="s">
         <v>225</v>
       </c>
@@ -15601,7 +15661,7 @@
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1">
       <c r="A15" s="19"/>
-      <c r="B15" s="58"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="19" t="s">
         <v>228</v>
       </c>

</xml_diff>